<commit_message>
Build tool steer form for settings
</commit_message>
<xml_diff>
--- a/SourceCode/AOG/Translations.xlsx
+++ b/SourceCode/AOG/Translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6403" uniqueCount="6055">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6406" uniqueCount="6058">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -16946,6 +16946,33 @@
     <t xml:space="preserve">Meni mašine</t>
   </si>
   <si>
+    <t xml:space="preserve">gsToolSteerConfiguration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tools Steer Configuration</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tools Steer Configuration</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">gsTopFieldView</t>
   </si>
   <si>
@@ -18712,7 +18739,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -18741,6 +18768,18 @@
       <name val="Microsoft YaHei"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
+      <name val="Cascadia Mono"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -18785,7 +18824,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -18799,6 +18838,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -19005,9 +19048,9 @@
   <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A322" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A214" activeCellId="0" sqref="A214"/>
+      <selection pane="bottomLeft" activeCell="D339" activeCellId="0" sqref="D339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -37146,1932 +37189,1954 @@
       </c>
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A339" s="2" t="s">
+      <c r="A339" s="4" t="s">
         <v>5488</v>
       </c>
       <c r="C339" s="2" t="s">
         <v>5489</v>
       </c>
-      <c r="D339" s="2" t="s">
+      <c r="D339" s="1" t="s">
         <v>5490</v>
       </c>
-      <c r="E339" s="2" t="s">
-        <v>5491</v>
-      </c>
-      <c r="F339" s="2" t="s">
-        <v>5492</v>
-      </c>
-      <c r="G339" s="2" t="s">
-        <v>5493</v>
-      </c>
-      <c r="H339" s="2" t="s">
-        <v>5494</v>
-      </c>
-      <c r="I339" s="2" t="s">
-        <v>5495</v>
-      </c>
-      <c r="J339" s="2" t="s">
-        <v>5496</v>
-      </c>
-      <c r="K339" s="2" t="s">
-        <v>5497</v>
-      </c>
-      <c r="L339" s="2" t="s">
-        <v>5498</v>
-      </c>
-      <c r="M339" s="2" t="s">
-        <v>5499</v>
-      </c>
-      <c r="N339" s="2" t="s">
-        <v>5500</v>
-      </c>
-      <c r="O339" s="2" t="s">
-        <v>5501</v>
-      </c>
-      <c r="P339" s="2" t="s">
-        <v>5502</v>
-      </c>
-      <c r="Q339" s="2" t="s">
-        <v>5503</v>
-      </c>
-      <c r="R339" s="2" t="s">
-        <v>5504</v>
-      </c>
-      <c r="S339" s="2" t="s">
-        <v>5505</v>
-      </c>
-      <c r="T339" s="2" t="s">
-        <v>5506</v>
-      </c>
-      <c r="U339" s="2" t="s">
-        <v>5507</v>
-      </c>
-      <c r="V339" s="2" t="s">
-        <v>5508</v>
-      </c>
-      <c r="W339" s="3" t="s">
-        <v>5509</v>
-      </c>
+      <c r="E339" s="2"/>
+      <c r="F339" s="2"/>
+      <c r="H339" s="2"/>
+      <c r="I339" s="2"/>
+      <c r="J339" s="2"/>
+      <c r="K339" s="2"/>
+      <c r="L339" s="2"/>
+      <c r="M339" s="2"/>
+      <c r="N339" s="2"/>
+      <c r="O339" s="2"/>
+      <c r="P339" s="2"/>
+      <c r="T339" s="2"/>
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="2" t="s">
+        <v>5491</v>
+      </c>
+      <c r="C340" s="2" t="s">
+        <v>5492</v>
+      </c>
+      <c r="D340" s="2" t="s">
+        <v>5493</v>
+      </c>
+      <c r="E340" s="2" t="s">
+        <v>5494</v>
+      </c>
+      <c r="F340" s="2" t="s">
+        <v>5495</v>
+      </c>
+      <c r="G340" s="2" t="s">
+        <v>5496</v>
+      </c>
+      <c r="H340" s="2" t="s">
+        <v>5497</v>
+      </c>
+      <c r="I340" s="2" t="s">
+        <v>5498</v>
+      </c>
+      <c r="J340" s="2" t="s">
+        <v>5499</v>
+      </c>
+      <c r="K340" s="2" t="s">
+        <v>5500</v>
+      </c>
+      <c r="L340" s="2" t="s">
+        <v>5501</v>
+      </c>
+      <c r="M340" s="2" t="s">
+        <v>5502</v>
+      </c>
+      <c r="N340" s="2" t="s">
+        <v>5503</v>
+      </c>
+      <c r="O340" s="2" t="s">
+        <v>5504</v>
+      </c>
+      <c r="P340" s="2" t="s">
+        <v>5505</v>
+      </c>
+      <c r="Q340" s="2" t="s">
+        <v>5506</v>
+      </c>
+      <c r="R340" s="2" t="s">
+        <v>5507</v>
+      </c>
+      <c r="S340" s="2" t="s">
+        <v>5508</v>
+      </c>
+      <c r="T340" s="2" t="s">
+        <v>5509</v>
+      </c>
+      <c r="U340" s="2" t="s">
         <v>5510</v>
       </c>
-      <c r="C340" s="2" t="s">
+      <c r="V340" s="2" t="s">
         <v>5511</v>
       </c>
-      <c r="D340" s="1" t="s">
+      <c r="W340" s="3" t="s">
         <v>5512</v>
-      </c>
-      <c r="H340" s="2" t="s">
-        <v>5513</v>
-      </c>
-      <c r="I340" s="2" t="s">
-        <v>5511</v>
-      </c>
-      <c r="J340" s="2" t="s">
-        <v>5514</v>
-      </c>
-      <c r="K340" s="2" t="s">
-        <v>5515</v>
-      </c>
-      <c r="L340" s="2" t="s">
-        <v>5516</v>
-      </c>
-      <c r="M340" s="2" t="s">
-        <v>5517</v>
-      </c>
-      <c r="N340" s="2" t="s">
-        <v>5518</v>
-      </c>
-      <c r="O340" s="2" t="s">
-        <v>5519</v>
-      </c>
-      <c r="T340" s="2" t="s">
-        <v>5520</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="2" t="s">
+        <v>5513</v>
+      </c>
+      <c r="C341" s="2" t="s">
+        <v>5514</v>
+      </c>
+      <c r="D341" s="1" t="s">
+        <v>5515</v>
+      </c>
+      <c r="H341" s="2" t="s">
+        <v>5516</v>
+      </c>
+      <c r="I341" s="2" t="s">
+        <v>5514</v>
+      </c>
+      <c r="J341" s="2" t="s">
+        <v>5517</v>
+      </c>
+      <c r="K341" s="2" t="s">
+        <v>5518</v>
+      </c>
+      <c r="L341" s="2" t="s">
+        <v>5519</v>
+      </c>
+      <c r="M341" s="2" t="s">
+        <v>5520</v>
+      </c>
+      <c r="N341" s="2" t="s">
         <v>5521</v>
       </c>
-      <c r="C341" s="2" t="s">
+      <c r="O341" s="2" t="s">
         <v>5522</v>
       </c>
-      <c r="D341" s="1" t="s">
+      <c r="T341" s="2" t="s">
         <v>5523</v>
-      </c>
-      <c r="E341" s="2" t="s">
-        <v>5524</v>
-      </c>
-      <c r="F341" s="2" t="s">
-        <v>5525</v>
-      </c>
-      <c r="H341" s="2" t="s">
-        <v>5526</v>
-      </c>
-      <c r="I341" s="2" t="s">
-        <v>5527</v>
-      </c>
-      <c r="J341" s="2" t="s">
-        <v>5528</v>
-      </c>
-      <c r="K341" s="2" t="s">
-        <v>5529</v>
-      </c>
-      <c r="L341" s="2" t="s">
-        <v>5530</v>
-      </c>
-      <c r="M341" s="2" t="s">
-        <v>5531</v>
-      </c>
-      <c r="N341" s="2" t="s">
-        <v>5532</v>
-      </c>
-      <c r="O341" s="2" t="s">
-        <v>5533</v>
-      </c>
-      <c r="R341" s="2" t="s">
-        <v>5534</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="2" t="s">
+        <v>5524</v>
+      </c>
+      <c r="C342" s="2" t="s">
+        <v>5525</v>
+      </c>
+      <c r="D342" s="1" t="s">
+        <v>5526</v>
+      </c>
+      <c r="E342" s="2" t="s">
+        <v>5527</v>
+      </c>
+      <c r="F342" s="2" t="s">
+        <v>5528</v>
+      </c>
+      <c r="H342" s="2" t="s">
+        <v>5529</v>
+      </c>
+      <c r="I342" s="2" t="s">
+        <v>5530</v>
+      </c>
+      <c r="J342" s="2" t="s">
+        <v>5531</v>
+      </c>
+      <c r="K342" s="2" t="s">
+        <v>5532</v>
+      </c>
+      <c r="L342" s="2" t="s">
+        <v>5533</v>
+      </c>
+      <c r="M342" s="2" t="s">
+        <v>5534</v>
+      </c>
+      <c r="N342" s="2" t="s">
         <v>5535</v>
       </c>
-      <c r="C342" s="2" t="s">
+      <c r="O342" s="2" t="s">
         <v>5536</v>
       </c>
-      <c r="D342" s="1" t="s">
+      <c r="R342" s="2" t="s">
         <v>5537</v>
-      </c>
-      <c r="E342" s="2" t="s">
-        <v>5538</v>
-      </c>
-      <c r="F342" s="2" t="s">
-        <v>5539</v>
-      </c>
-      <c r="H342" s="2" t="s">
-        <v>5540</v>
-      </c>
-      <c r="I342" s="2" t="s">
-        <v>5541</v>
-      </c>
-      <c r="J342" s="2" t="s">
-        <v>5542</v>
-      </c>
-      <c r="K342" s="2" t="s">
-        <v>5543</v>
-      </c>
-      <c r="L342" s="2" t="s">
-        <v>5544</v>
-      </c>
-      <c r="M342" s="2" t="s">
-        <v>5545</v>
-      </c>
-      <c r="N342" s="2" t="s">
-        <v>5546</v>
-      </c>
-      <c r="O342" s="2" t="s">
-        <v>5533</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="2" t="s">
+        <v>5538</v>
+      </c>
+      <c r="C343" s="2" t="s">
+        <v>5539</v>
+      </c>
+      <c r="D343" s="1" t="s">
+        <v>5540</v>
+      </c>
+      <c r="E343" s="2" t="s">
+        <v>5541</v>
+      </c>
+      <c r="F343" s="2" t="s">
+        <v>5542</v>
+      </c>
+      <c r="H343" s="2" t="s">
+        <v>5543</v>
+      </c>
+      <c r="I343" s="2" t="s">
+        <v>5544</v>
+      </c>
+      <c r="J343" s="2" t="s">
+        <v>5545</v>
+      </c>
+      <c r="K343" s="2" t="s">
+        <v>5546</v>
+      </c>
+      <c r="L343" s="2" t="s">
         <v>5547</v>
       </c>
-      <c r="C343" s="2" t="s">
+      <c r="M343" s="2" t="s">
         <v>5548</v>
       </c>
-      <c r="D343" s="2" t="s">
+      <c r="N343" s="2" t="s">
         <v>5549</v>
       </c>
-      <c r="E343" s="2" t="s">
-        <v>5550</v>
-      </c>
-      <c r="F343" s="2" t="s">
-        <v>4889</v>
-      </c>
-      <c r="G343" s="2" t="s">
-        <v>5551</v>
-      </c>
-      <c r="H343" s="2" t="s">
-        <v>5552</v>
-      </c>
-      <c r="I343" s="2" t="s">
-        <v>5553</v>
-      </c>
-      <c r="J343" s="2" t="s">
-        <v>5554</v>
-      </c>
-      <c r="K343" s="2" t="s">
-        <v>5555</v>
-      </c>
-      <c r="L343" s="2" t="s">
-        <v>5556</v>
-      </c>
-      <c r="M343" s="2" t="s">
-        <v>5557</v>
-      </c>
-      <c r="N343" s="2" t="s">
-        <v>5558</v>
-      </c>
       <c r="O343" s="2" t="s">
-        <v>5559</v>
-      </c>
-      <c r="P343" s="2" t="s">
-        <v>5560</v>
-      </c>
-      <c r="Q343" s="2" t="s">
-        <v>5561</v>
-      </c>
-      <c r="R343" s="2" t="s">
-        <v>5562</v>
-      </c>
-      <c r="S343" s="2" t="s">
-        <v>5563</v>
-      </c>
-      <c r="U343" s="2" t="s">
-        <v>5564</v>
-      </c>
-      <c r="V343" s="2" t="s">
-        <v>5565</v>
-      </c>
-      <c r="W343" s="3" t="s">
-        <v>5566</v>
+        <v>5536</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="2" t="s">
+        <v>5550</v>
+      </c>
+      <c r="C344" s="2" t="s">
+        <v>5551</v>
+      </c>
+      <c r="D344" s="2" t="s">
+        <v>5552</v>
+      </c>
+      <c r="E344" s="2" t="s">
+        <v>5553</v>
+      </c>
+      <c r="F344" s="2" t="s">
+        <v>4889</v>
+      </c>
+      <c r="G344" s="2" t="s">
+        <v>5554</v>
+      </c>
+      <c r="H344" s="2" t="s">
+        <v>5555</v>
+      </c>
+      <c r="I344" s="2" t="s">
+        <v>5556</v>
+      </c>
+      <c r="J344" s="2" t="s">
+        <v>5557</v>
+      </c>
+      <c r="K344" s="2" t="s">
+        <v>5558</v>
+      </c>
+      <c r="L344" s="2" t="s">
+        <v>5559</v>
+      </c>
+      <c r="M344" s="2" t="s">
+        <v>5560</v>
+      </c>
+      <c r="N344" s="2" t="s">
+        <v>5561</v>
+      </c>
+      <c r="O344" s="2" t="s">
+        <v>5562</v>
+      </c>
+      <c r="P344" s="2" t="s">
+        <v>5563</v>
+      </c>
+      <c r="Q344" s="2" t="s">
+        <v>5564</v>
+      </c>
+      <c r="R344" s="2" t="s">
+        <v>5565</v>
+      </c>
+      <c r="S344" s="2" t="s">
+        <v>5566</v>
+      </c>
+      <c r="U344" s="2" t="s">
         <v>5567</v>
       </c>
-      <c r="C344" s="2" t="s">
+      <c r="V344" s="2" t="s">
         <v>5568</v>
       </c>
-      <c r="D344" s="1" t="s">
+      <c r="W344" s="3" t="s">
         <v>5569</v>
       </c>
-      <c r="E344" s="2" t="s">
+    </row>
+    <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="2" t="s">
         <v>5570</v>
       </c>
-      <c r="F344" s="2" t="s">
+      <c r="C345" s="2" t="s">
         <v>5571</v>
       </c>
-      <c r="H344" s="2" t="s">
+      <c r="D345" s="1" t="s">
         <v>5572</v>
       </c>
-      <c r="I344" s="2" t="s">
+      <c r="E345" s="2" t="s">
         <v>5573</v>
       </c>
-      <c r="J344" s="2" t="s">
+      <c r="F345" s="2" t="s">
         <v>5574</v>
       </c>
-      <c r="K344" s="2" t="s">
+      <c r="H345" s="2" t="s">
         <v>5575</v>
       </c>
-      <c r="L344" s="2" t="s">
+      <c r="I345" s="2" t="s">
         <v>5576</v>
       </c>
-      <c r="M344" s="2" t="s">
+      <c r="J345" s="2" t="s">
         <v>5577</v>
       </c>
-      <c r="N344" s="2" t="s">
+      <c r="K345" s="2" t="s">
         <v>5578</v>
       </c>
-      <c r="O344" s="2" t="s">
+      <c r="L345" s="2" t="s">
         <v>5579</v>
       </c>
-      <c r="R344" s="2" t="s">
+      <c r="M345" s="2" t="s">
         <v>5580</v>
       </c>
+      <c r="N345" s="2" t="s">
+        <v>5581</v>
+      </c>
+      <c r="O345" s="2" t="s">
+        <v>5582</v>
+      </c>
+      <c r="R345" s="2" t="s">
+        <v>5583</v>
+      </c>
     </row>
-    <row r="345" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A345" s="2" t="s">
-        <v>5581</v>
-      </c>
-      <c r="C345" s="2" t="s">
-        <v>5582</v>
-      </c>
-      <c r="D345" s="2" t="s">
-        <v>5583</v>
-      </c>
-      <c r="E345" s="2" t="s">
+    <row r="346" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A346" s="2" t="s">
         <v>5584</v>
       </c>
-      <c r="F345" s="2" t="s">
+      <c r="C346" s="2" t="s">
         <v>5585</v>
       </c>
-      <c r="G345" s="2" t="s">
+      <c r="D346" s="2" t="s">
         <v>5586</v>
       </c>
-      <c r="H345" s="2" t="s">
+      <c r="E346" s="2" t="s">
         <v>5587</v>
       </c>
-      <c r="I345" s="2" t="s">
+      <c r="F346" s="2" t="s">
         <v>5588</v>
       </c>
-      <c r="J345" s="2" t="s">
+      <c r="G346" s="2" t="s">
         <v>5589</v>
       </c>
-      <c r="K345" s="2" t="s">
+      <c r="H346" s="2" t="s">
         <v>5590</v>
       </c>
-      <c r="L345" s="2" t="s">
+      <c r="I346" s="2" t="s">
         <v>5591</v>
       </c>
-      <c r="M345" s="2" t="s">
+      <c r="J346" s="2" t="s">
         <v>5592</v>
       </c>
-      <c r="N345" s="2" t="s">
+      <c r="K346" s="2" t="s">
         <v>5593</v>
       </c>
-      <c r="O345" s="2" t="s">
+      <c r="L346" s="2" t="s">
         <v>5594</v>
       </c>
-      <c r="P345" s="2" t="s">
+      <c r="M346" s="2" t="s">
         <v>5595</v>
       </c>
-      <c r="Q345" s="2" t="s">
+      <c r="N346" s="2" t="s">
         <v>5596</v>
       </c>
-      <c r="R345" s="2" t="s">
+      <c r="O346" s="2" t="s">
         <v>5597</v>
       </c>
-      <c r="S345" s="2" t="s">
+      <c r="P346" s="2" t="s">
         <v>5598</v>
       </c>
-      <c r="T345" s="2" t="s">
+      <c r="Q346" s="2" t="s">
         <v>5599</v>
       </c>
-      <c r="U345" s="2" t="s">
+      <c r="R346" s="2" t="s">
         <v>5600</v>
       </c>
-      <c r="V345" s="2" t="s">
+      <c r="S346" s="2" t="s">
         <v>5601</v>
       </c>
-      <c r="W345" s="3" t="s">
+      <c r="T346" s="2" t="s">
         <v>5602</v>
       </c>
-    </row>
-    <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A346" s="2" t="s">
+      <c r="U346" s="2" t="s">
         <v>5603</v>
       </c>
-      <c r="C346" s="2" t="s">
+      <c r="V346" s="2" t="s">
         <v>5604</v>
       </c>
-      <c r="D346" s="1" t="s">
+      <c r="W346" s="3" t="s">
         <v>5605</v>
-      </c>
-      <c r="F346" s="2" t="s">
-        <v>5606</v>
-      </c>
-      <c r="H346" s="2" t="s">
-        <v>5607</v>
-      </c>
-      <c r="I346" s="2" t="s">
-        <v>5608</v>
-      </c>
-      <c r="J346" s="2" t="s">
-        <v>5609</v>
-      </c>
-      <c r="K346" s="2" t="s">
-        <v>5610</v>
-      </c>
-      <c r="L346" s="2" t="s">
-        <v>5611</v>
-      </c>
-      <c r="M346" s="2" t="s">
-        <v>5612</v>
-      </c>
-      <c r="N346" s="2" t="s">
-        <v>5613</v>
-      </c>
-      <c r="O346" s="2" t="s">
-        <v>5614</v>
-      </c>
-      <c r="R346" s="2" t="s">
-        <v>5615</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="2" t="s">
+        <v>5606</v>
+      </c>
+      <c r="C347" s="2" t="s">
+        <v>5607</v>
+      </c>
+      <c r="D347" s="1" t="s">
+        <v>5608</v>
+      </c>
+      <c r="F347" s="2" t="s">
+        <v>5609</v>
+      </c>
+      <c r="H347" s="2" t="s">
+        <v>5610</v>
+      </c>
+      <c r="I347" s="2" t="s">
+        <v>5611</v>
+      </c>
+      <c r="J347" s="2" t="s">
+        <v>5612</v>
+      </c>
+      <c r="K347" s="2" t="s">
+        <v>5613</v>
+      </c>
+      <c r="L347" s="2" t="s">
+        <v>5614</v>
+      </c>
+      <c r="M347" s="2" t="s">
+        <v>5615</v>
+      </c>
+      <c r="N347" s="2" t="s">
         <v>5616</v>
       </c>
-      <c r="C347" s="2" t="s">
+      <c r="O347" s="2" t="s">
         <v>5617</v>
       </c>
-      <c r="D347" s="1" t="s">
+      <c r="R347" s="2" t="s">
         <v>5618</v>
       </c>
-      <c r="F347" s="2" t="s">
+    </row>
+    <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A348" s="2" t="s">
         <v>5619</v>
       </c>
-      <c r="H347" s="2" t="s">
+      <c r="C348" s="2" t="s">
         <v>5620</v>
       </c>
-      <c r="J347" s="2" t="s">
+      <c r="D348" s="1" t="s">
         <v>5621</v>
       </c>
-      <c r="K347" s="2" t="s">
+      <c r="F348" s="2" t="s">
         <v>5622</v>
       </c>
-      <c r="L347" s="2" t="s">
+      <c r="H348" s="2" t="s">
         <v>5623</v>
       </c>
-      <c r="M347" s="2" t="s">
+      <c r="J348" s="2" t="s">
         <v>5624</v>
       </c>
-      <c r="N347" s="2" t="s">
+      <c r="K348" s="2" t="s">
         <v>5625</v>
       </c>
-      <c r="O347" s="2" t="s">
+      <c r="L348" s="2" t="s">
         <v>5626</v>
       </c>
-      <c r="R347" s="2" t="s">
+      <c r="M348" s="2" t="s">
         <v>5627</v>
       </c>
+      <c r="N348" s="2" t="s">
+        <v>5628</v>
+      </c>
+      <c r="O348" s="2" t="s">
+        <v>5629</v>
+      </c>
+      <c r="R348" s="2" t="s">
+        <v>5630</v>
+      </c>
     </row>
-    <row r="348" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A348" s="2" t="s">
-        <v>5628</v>
-      </c>
-      <c r="C348" s="2" t="s">
-        <v>5629</v>
-      </c>
-      <c r="D348" s="2" t="s">
-        <v>5630</v>
-      </c>
-      <c r="E348" s="2" t="s">
+    <row r="349" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A349" s="2" t="s">
         <v>5631</v>
       </c>
-      <c r="F348" s="2" t="s">
+      <c r="C349" s="2" t="s">
         <v>5632</v>
       </c>
-      <c r="G348" s="2" t="s">
+      <c r="D349" s="2" t="s">
         <v>5633</v>
       </c>
-      <c r="H348" s="2" t="s">
+      <c r="E349" s="2" t="s">
         <v>5634</v>
       </c>
-      <c r="I348" s="2" t="s">
+      <c r="F349" s="2" t="s">
         <v>5635</v>
       </c>
-      <c r="J348" s="2" t="s">
+      <c r="G349" s="2" t="s">
         <v>5636</v>
       </c>
-      <c r="K348" s="2" t="s">
+      <c r="H349" s="2" t="s">
         <v>5637</v>
       </c>
-      <c r="L348" s="2" t="s">
+      <c r="I349" s="2" t="s">
         <v>5638</v>
       </c>
-      <c r="M348" s="2" t="s">
+      <c r="J349" s="2" t="s">
         <v>5639</v>
       </c>
-      <c r="N348" s="2" t="s">
+      <c r="K349" s="2" t="s">
         <v>5640</v>
       </c>
-      <c r="O348" s="2" t="s">
+      <c r="L349" s="2" t="s">
         <v>5641</v>
       </c>
-      <c r="P348" s="2" t="s">
+      <c r="M349" s="2" t="s">
         <v>5642</v>
       </c>
-      <c r="Q348" s="2" t="s">
+      <c r="N349" s="2" t="s">
         <v>5643</v>
       </c>
-      <c r="R348" s="2" t="s">
+      <c r="O349" s="2" t="s">
         <v>5644</v>
       </c>
-      <c r="S348" s="2" t="s">
+      <c r="P349" s="2" t="s">
         <v>5645</v>
       </c>
-      <c r="U348" s="2" t="s">
+      <c r="Q349" s="2" t="s">
         <v>5646</v>
       </c>
-      <c r="V348" s="2" t="s">
+      <c r="R349" s="2" t="s">
         <v>5647</v>
       </c>
-      <c r="W348" s="3" t="s">
+      <c r="S349" s="2" t="s">
         <v>5648</v>
       </c>
-    </row>
-    <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A349" s="2" t="s">
+      <c r="U349" s="2" t="s">
         <v>5649</v>
       </c>
-      <c r="C349" s="2" t="s">
+      <c r="V349" s="2" t="s">
         <v>5650</v>
       </c>
-      <c r="D349" s="1" t="s">
+      <c r="W349" s="3" t="s">
         <v>5651</v>
-      </c>
-      <c r="F349" s="2" t="s">
-        <v>5652</v>
-      </c>
-      <c r="H349" s="2" t="s">
-        <v>5653</v>
-      </c>
-      <c r="I349" s="2" t="s">
-        <v>5654</v>
-      </c>
-      <c r="J349" s="2" t="s">
-        <v>1263</v>
-      </c>
-      <c r="K349" s="2" t="s">
-        <v>5655</v>
-      </c>
-      <c r="L349" s="2" t="s">
-        <v>5656</v>
-      </c>
-      <c r="M349" s="2" t="s">
-        <v>5657</v>
-      </c>
-      <c r="N349" s="2" t="s">
-        <v>5658</v>
-      </c>
-      <c r="O349" s="2" t="s">
-        <v>5659</v>
-      </c>
-      <c r="P349" s="2" t="s">
-        <v>1269</v>
-      </c>
-      <c r="T349" s="2" t="s">
-        <v>5660</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="2" t="s">
+        <v>5652</v>
+      </c>
+      <c r="C350" s="2" t="s">
+        <v>5653</v>
+      </c>
+      <c r="D350" s="1" t="s">
+        <v>5654</v>
+      </c>
+      <c r="F350" s="2" t="s">
+        <v>5655</v>
+      </c>
+      <c r="H350" s="2" t="s">
+        <v>5656</v>
+      </c>
+      <c r="I350" s="2" t="s">
+        <v>5657</v>
+      </c>
+      <c r="J350" s="2" t="s">
+        <v>1263</v>
+      </c>
+      <c r="K350" s="2" t="s">
+        <v>5658</v>
+      </c>
+      <c r="L350" s="2" t="s">
+        <v>5659</v>
+      </c>
+      <c r="M350" s="2" t="s">
+        <v>5660</v>
+      </c>
+      <c r="N350" s="2" t="s">
         <v>5661</v>
       </c>
-      <c r="C350" s="2" t="s">
+      <c r="O350" s="2" t="s">
         <v>5662</v>
       </c>
-      <c r="D350" s="1" t="s">
+      <c r="P350" s="2" t="s">
+        <v>1269</v>
+      </c>
+      <c r="T350" s="2" t="s">
         <v>5663</v>
-      </c>
-      <c r="F350" s="2" t="s">
-        <v>5664</v>
-      </c>
-      <c r="H350" s="2" t="s">
-        <v>5665</v>
-      </c>
-      <c r="I350" s="2" t="s">
-        <v>5666</v>
-      </c>
-      <c r="J350" s="2" t="s">
-        <v>5667</v>
-      </c>
-      <c r="K350" s="2" t="s">
-        <v>5668</v>
-      </c>
-      <c r="L350" s="2" t="s">
-        <v>5669</v>
-      </c>
-      <c r="M350" s="2" t="s">
-        <v>5670</v>
-      </c>
-      <c r="N350" s="2" t="s">
-        <v>5671</v>
-      </c>
-      <c r="O350" s="2" t="s">
-        <v>5672</v>
-      </c>
-      <c r="P350" s="2" t="s">
-        <v>5673</v>
-      </c>
-      <c r="T350" s="2" t="s">
-        <v>5674</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="2" t="s">
+        <v>5664</v>
+      </c>
+      <c r="C351" s="2" t="s">
+        <v>5665</v>
+      </c>
+      <c r="D351" s="1" t="s">
+        <v>5666</v>
+      </c>
+      <c r="F351" s="2" t="s">
+        <v>5667</v>
+      </c>
+      <c r="H351" s="2" t="s">
+        <v>5668</v>
+      </c>
+      <c r="I351" s="2" t="s">
+        <v>5669</v>
+      </c>
+      <c r="J351" s="2" t="s">
+        <v>5670</v>
+      </c>
+      <c r="K351" s="2" t="s">
+        <v>5671</v>
+      </c>
+      <c r="L351" s="2" t="s">
+        <v>5672</v>
+      </c>
+      <c r="M351" s="2" t="s">
+        <v>5673</v>
+      </c>
+      <c r="N351" s="2" t="s">
+        <v>5674</v>
+      </c>
+      <c r="O351" s="2" t="s">
         <v>5675</v>
       </c>
-      <c r="C351" s="2" t="s">
+      <c r="P351" s="2" t="s">
         <v>5676</v>
       </c>
-      <c r="D351" s="1" t="s">
+      <c r="T351" s="2" t="s">
         <v>5677</v>
-      </c>
-      <c r="F351" s="2" t="s">
-        <v>5678</v>
-      </c>
-      <c r="H351" s="2" t="s">
-        <v>5679</v>
-      </c>
-      <c r="I351" s="2" t="s">
-        <v>5666</v>
-      </c>
-      <c r="J351" s="2" t="s">
-        <v>5680</v>
-      </c>
-      <c r="K351" s="2" t="s">
-        <v>5668</v>
-      </c>
-      <c r="L351" s="2" t="s">
-        <v>5681</v>
-      </c>
-      <c r="M351" s="2" t="s">
-        <v>5682</v>
-      </c>
-      <c r="N351" s="2" t="s">
-        <v>5683</v>
-      </c>
-      <c r="O351" s="2" t="s">
-        <v>5684</v>
-      </c>
-      <c r="P351" s="2" t="s">
-        <v>5685</v>
-      </c>
-      <c r="T351" s="2" t="s">
-        <v>5686</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="2" t="s">
+        <v>5678</v>
+      </c>
+      <c r="C352" s="2" t="s">
+        <v>5679</v>
+      </c>
+      <c r="D352" s="1" t="s">
+        <v>5680</v>
+      </c>
+      <c r="F352" s="2" t="s">
+        <v>5681</v>
+      </c>
+      <c r="H352" s="2" t="s">
+        <v>5682</v>
+      </c>
+      <c r="I352" s="2" t="s">
+        <v>5669</v>
+      </c>
+      <c r="J352" s="2" t="s">
+        <v>5683</v>
+      </c>
+      <c r="K352" s="2" t="s">
+        <v>5671</v>
+      </c>
+      <c r="L352" s="2" t="s">
+        <v>5684</v>
+      </c>
+      <c r="M352" s="2" t="s">
+        <v>5685</v>
+      </c>
+      <c r="N352" s="2" t="s">
+        <v>5686</v>
+      </c>
+      <c r="O352" s="2" t="s">
         <v>5687</v>
       </c>
-      <c r="C352" s="2" t="s">
+      <c r="P352" s="2" t="s">
         <v>5688</v>
       </c>
-      <c r="D352" s="2" t="s">
+      <c r="T352" s="2" t="s">
         <v>5689</v>
-      </c>
-      <c r="E352" s="2" t="s">
-        <v>5690</v>
-      </c>
-      <c r="F352" s="2" t="s">
-        <v>5691</v>
-      </c>
-      <c r="G352" s="2" t="s">
-        <v>5692</v>
-      </c>
-      <c r="H352" s="2" t="s">
-        <v>5693</v>
-      </c>
-      <c r="I352" s="2" t="s">
-        <v>5694</v>
-      </c>
-      <c r="J352" s="2" t="s">
-        <v>3848</v>
-      </c>
-      <c r="K352" s="2" t="s">
-        <v>5695</v>
-      </c>
-      <c r="L352" s="2" t="s">
-        <v>5696</v>
-      </c>
-      <c r="M352" s="2" t="s">
-        <v>5697</v>
-      </c>
-      <c r="N352" s="2" t="s">
-        <v>5698</v>
-      </c>
-      <c r="O352" s="2" t="s">
-        <v>5699</v>
-      </c>
-      <c r="P352" s="2" t="s">
-        <v>5700</v>
-      </c>
-      <c r="Q352" s="2" t="s">
-        <v>5701</v>
-      </c>
-      <c r="R352" s="2" t="s">
-        <v>5702</v>
-      </c>
-      <c r="S352" s="2" t="s">
-        <v>5703</v>
-      </c>
-      <c r="T352" s="2" t="s">
-        <v>5704</v>
-      </c>
-      <c r="U352" s="2" t="s">
-        <v>5705</v>
-      </c>
-      <c r="V352" s="2" t="s">
-        <v>5706</v>
-      </c>
-      <c r="W352" s="3" t="s">
-        <v>5707</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="2" t="s">
+        <v>5690</v>
+      </c>
+      <c r="C353" s="2" t="s">
+        <v>5691</v>
+      </c>
+      <c r="D353" s="2" t="s">
+        <v>5692</v>
+      </c>
+      <c r="E353" s="2" t="s">
+        <v>5693</v>
+      </c>
+      <c r="F353" s="2" t="s">
+        <v>5694</v>
+      </c>
+      <c r="G353" s="2" t="s">
+        <v>5695</v>
+      </c>
+      <c r="H353" s="2" t="s">
+        <v>5696</v>
+      </c>
+      <c r="I353" s="2" t="s">
+        <v>5697</v>
+      </c>
+      <c r="J353" s="2" t="s">
+        <v>3848</v>
+      </c>
+      <c r="K353" s="2" t="s">
+        <v>5698</v>
+      </c>
+      <c r="L353" s="2" t="s">
+        <v>5699</v>
+      </c>
+      <c r="M353" s="2" t="s">
+        <v>5700</v>
+      </c>
+      <c r="N353" s="2" t="s">
+        <v>5701</v>
+      </c>
+      <c r="O353" s="2" t="s">
+        <v>5702</v>
+      </c>
+      <c r="P353" s="2" t="s">
+        <v>5703</v>
+      </c>
+      <c r="Q353" s="2" t="s">
+        <v>5704</v>
+      </c>
+      <c r="R353" s="2" t="s">
+        <v>5705</v>
+      </c>
+      <c r="S353" s="2" t="s">
+        <v>5706</v>
+      </c>
+      <c r="T353" s="2" t="s">
+        <v>5707</v>
+      </c>
+      <c r="U353" s="2" t="s">
         <v>5708</v>
       </c>
-      <c r="C353" s="2" t="s">
+      <c r="V353" s="2" t="s">
         <v>5709</v>
       </c>
-      <c r="D353" s="1" t="s">
+      <c r="W353" s="3" t="s">
         <v>5710</v>
-      </c>
-      <c r="H353" s="2" t="s">
-        <v>5711</v>
-      </c>
-      <c r="I353" s="2" t="s">
-        <v>5712</v>
-      </c>
-      <c r="J353" s="2" t="s">
-        <v>5713</v>
-      </c>
-      <c r="K353" s="2" t="s">
-        <v>5714</v>
-      </c>
-      <c r="L353" s="2" t="s">
-        <v>5715</v>
-      </c>
-      <c r="M353" s="2" t="s">
-        <v>5716</v>
-      </c>
-      <c r="O353" s="2" t="s">
-        <v>5717</v>
-      </c>
-      <c r="P353" s="2" t="s">
-        <v>5709</v>
-      </c>
-      <c r="T353" s="2" t="s">
-        <v>5718</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="2" t="s">
+        <v>5711</v>
+      </c>
+      <c r="C354" s="2" t="s">
+        <v>5712</v>
+      </c>
+      <c r="D354" s="1" t="s">
+        <v>5713</v>
+      </c>
+      <c r="H354" s="2" t="s">
+        <v>5714</v>
+      </c>
+      <c r="I354" s="2" t="s">
+        <v>5715</v>
+      </c>
+      <c r="J354" s="2" t="s">
+        <v>5716</v>
+      </c>
+      <c r="K354" s="2" t="s">
+        <v>5717</v>
+      </c>
+      <c r="L354" s="2" t="s">
+        <v>5718</v>
+      </c>
+      <c r="M354" s="2" t="s">
         <v>5719</v>
       </c>
-      <c r="C354" s="2" t="s">
+      <c r="O354" s="2" t="s">
         <v>5720</v>
       </c>
-      <c r="D354" s="1" t="s">
+      <c r="P354" s="2" t="s">
+        <v>5712</v>
+      </c>
+      <c r="T354" s="2" t="s">
         <v>5721</v>
-      </c>
-      <c r="H354" s="2" t="s">
-        <v>5722</v>
-      </c>
-      <c r="I354" s="2" t="s">
-        <v>5723</v>
-      </c>
-      <c r="J354" s="2" t="s">
-        <v>5724</v>
-      </c>
-      <c r="K354" s="2" t="s">
-        <v>5725</v>
-      </c>
-      <c r="L354" s="2" t="s">
-        <v>5726</v>
-      </c>
-      <c r="M354" s="2" t="s">
-        <v>5727</v>
-      </c>
-      <c r="O354" s="2" t="s">
-        <v>5728</v>
-      </c>
-      <c r="P354" s="2" t="s">
-        <v>5720</v>
-      </c>
-      <c r="T354" s="2" t="s">
-        <v>5729</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="2" t="s">
+        <v>5722</v>
+      </c>
+      <c r="C355" s="2" t="s">
+        <v>5723</v>
+      </c>
+      <c r="D355" s="1" t="s">
+        <v>5724</v>
+      </c>
+      <c r="H355" s="2" t="s">
+        <v>5725</v>
+      </c>
+      <c r="I355" s="2" t="s">
+        <v>5726</v>
+      </c>
+      <c r="J355" s="2" t="s">
+        <v>5727</v>
+      </c>
+      <c r="K355" s="2" t="s">
+        <v>5728</v>
+      </c>
+      <c r="L355" s="2" t="s">
+        <v>5729</v>
+      </c>
+      <c r="M355" s="2" t="s">
         <v>5730</v>
       </c>
-      <c r="C355" s="2" t="s">
+      <c r="O355" s="2" t="s">
         <v>5731</v>
       </c>
-      <c r="D355" s="1" t="s">
+      <c r="P355" s="2" t="s">
+        <v>5723</v>
+      </c>
+      <c r="T355" s="2" t="s">
         <v>5732</v>
-      </c>
-      <c r="H355" s="2" t="s">
-        <v>5733</v>
-      </c>
-      <c r="I355" s="2" t="s">
-        <v>5734</v>
-      </c>
-      <c r="J355" s="2" t="s">
-        <v>5735</v>
-      </c>
-      <c r="K355" s="2" t="s">
-        <v>5736</v>
-      </c>
-      <c r="L355" s="2" t="s">
-        <v>5737</v>
-      </c>
-      <c r="M355" s="2" t="s">
-        <v>5738</v>
-      </c>
-      <c r="O355" s="2" t="s">
-        <v>5739</v>
-      </c>
-      <c r="P355" s="2" t="s">
-        <v>5731</v>
-      </c>
-      <c r="T355" s="2" t="s">
-        <v>5740</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="2" t="s">
+        <v>5733</v>
+      </c>
+      <c r="C356" s="2" t="s">
+        <v>5734</v>
+      </c>
+      <c r="D356" s="1" t="s">
+        <v>5735</v>
+      </c>
+      <c r="H356" s="2" t="s">
+        <v>5736</v>
+      </c>
+      <c r="I356" s="2" t="s">
+        <v>5737</v>
+      </c>
+      <c r="J356" s="2" t="s">
+        <v>5738</v>
+      </c>
+      <c r="K356" s="2" t="s">
+        <v>5739</v>
+      </c>
+      <c r="L356" s="2" t="s">
+        <v>5740</v>
+      </c>
+      <c r="M356" s="2" t="s">
         <v>5741</v>
       </c>
-      <c r="C356" s="2" t="s">
+      <c r="O356" s="2" t="s">
         <v>5742</v>
       </c>
-      <c r="D356" s="1" t="s">
+      <c r="P356" s="2" t="s">
+        <v>5734</v>
+      </c>
+      <c r="T356" s="2" t="s">
         <v>5743</v>
-      </c>
-      <c r="H356" s="2" t="s">
-        <v>5744</v>
-      </c>
-      <c r="I356" s="2" t="s">
-        <v>5745</v>
-      </c>
-      <c r="J356" s="2" t="s">
-        <v>5746</v>
-      </c>
-      <c r="K356" s="2" t="s">
-        <v>5747</v>
-      </c>
-      <c r="L356" s="2" t="s">
-        <v>5748</v>
-      </c>
-      <c r="M356" s="2" t="s">
-        <v>5749</v>
-      </c>
-      <c r="O356" s="2" t="s">
-        <v>5750</v>
-      </c>
-      <c r="P356" s="2" t="s">
-        <v>5742</v>
-      </c>
-      <c r="T356" s="2" t="s">
-        <v>5751</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="2" t="s">
+        <v>5744</v>
+      </c>
+      <c r="C357" s="2" t="s">
+        <v>5745</v>
+      </c>
+      <c r="D357" s="1" t="s">
+        <v>5746</v>
+      </c>
+      <c r="H357" s="2" t="s">
+        <v>5747</v>
+      </c>
+      <c r="I357" s="2" t="s">
+        <v>5748</v>
+      </c>
+      <c r="J357" s="2" t="s">
+        <v>5749</v>
+      </c>
+      <c r="K357" s="2" t="s">
+        <v>5750</v>
+      </c>
+      <c r="L357" s="2" t="s">
+        <v>5751</v>
+      </c>
+      <c r="M357" s="2" t="s">
         <v>5752</v>
       </c>
-      <c r="C357" s="2" t="s">
+      <c r="O357" s="2" t="s">
         <v>5753</v>
       </c>
-      <c r="D357" s="1" t="s">
+      <c r="P357" s="2" t="s">
+        <v>5745</v>
+      </c>
+      <c r="T357" s="2" t="s">
         <v>5754</v>
-      </c>
-      <c r="H357" s="2" t="s">
-        <v>5755</v>
-      </c>
-      <c r="I357" s="2" t="s">
-        <v>5753</v>
-      </c>
-      <c r="J357" s="2" t="s">
-        <v>5756</v>
-      </c>
-      <c r="K357" s="2" t="s">
-        <v>5757</v>
-      </c>
-      <c r="L357" s="2" t="s">
-        <v>5758</v>
-      </c>
-      <c r="M357" s="2" t="s">
-        <v>5759</v>
-      </c>
-      <c r="N357" s="2" t="s">
-        <v>5760</v>
-      </c>
-      <c r="O357" s="2" t="s">
-        <v>5761</v>
-      </c>
-      <c r="P357" s="2" t="s">
-        <v>5753</v>
-      </c>
-      <c r="R357" s="2" t="s">
-        <v>5762</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="2" t="s">
+        <v>5755</v>
+      </c>
+      <c r="C358" s="2" t="s">
+        <v>5756</v>
+      </c>
+      <c r="D358" s="1" t="s">
+        <v>5757</v>
+      </c>
+      <c r="H358" s="2" t="s">
+        <v>5758</v>
+      </c>
+      <c r="I358" s="2" t="s">
+        <v>5756</v>
+      </c>
+      <c r="J358" s="2" t="s">
+        <v>5759</v>
+      </c>
+      <c r="K358" s="2" t="s">
+        <v>5760</v>
+      </c>
+      <c r="L358" s="2" t="s">
+        <v>5761</v>
+      </c>
+      <c r="M358" s="2" t="s">
+        <v>5762</v>
+      </c>
+      <c r="N358" s="2" t="s">
         <v>5763</v>
       </c>
-      <c r="C358" s="2" t="s">
+      <c r="O358" s="2" t="s">
         <v>5764</v>
       </c>
-      <c r="D358" s="1" t="s">
+      <c r="P358" s="2" t="s">
+        <v>5756</v>
+      </c>
+      <c r="R358" s="2" t="s">
         <v>5765</v>
-      </c>
-      <c r="H358" s="2" t="s">
-        <v>5766</v>
-      </c>
-      <c r="I358" s="2" t="s">
-        <v>5764</v>
-      </c>
-      <c r="J358" s="2" t="s">
-        <v>5767</v>
-      </c>
-      <c r="K358" s="2" t="s">
-        <v>5768</v>
-      </c>
-      <c r="L358" s="2" t="s">
-        <v>5769</v>
-      </c>
-      <c r="M358" s="2" t="s">
-        <v>5770</v>
-      </c>
-      <c r="N358" s="2" t="s">
-        <v>5771</v>
-      </c>
-      <c r="O358" s="2" t="s">
-        <v>5772</v>
-      </c>
-      <c r="P358" s="2" t="s">
-        <v>5764</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="2" t="s">
+        <v>5766</v>
+      </c>
+      <c r="C359" s="2" t="s">
+        <v>5767</v>
+      </c>
+      <c r="D359" s="1" t="s">
+        <v>5768</v>
+      </c>
+      <c r="H359" s="2" t="s">
+        <v>5769</v>
+      </c>
+      <c r="I359" s="2" t="s">
+        <v>5767</v>
+      </c>
+      <c r="J359" s="2" t="s">
+        <v>5770</v>
+      </c>
+      <c r="K359" s="2" t="s">
+        <v>5771</v>
+      </c>
+      <c r="L359" s="2" t="s">
+        <v>5772</v>
+      </c>
+      <c r="M359" s="2" t="s">
         <v>5773</v>
       </c>
-      <c r="C359" s="2" t="s">
+      <c r="N359" s="2" t="s">
         <v>5774</v>
       </c>
-      <c r="D359" s="1" t="s">
+      <c r="O359" s="2" t="s">
         <v>5775</v>
       </c>
-      <c r="E359" s="2" t="s">
-        <v>5776</v>
-      </c>
-      <c r="F359" s="2" t="s">
-        <v>5777</v>
-      </c>
-      <c r="H359" s="2" t="s">
-        <v>5778</v>
-      </c>
-      <c r="I359" s="2" t="s">
-        <v>5779</v>
-      </c>
-      <c r="J359" s="2" t="s">
-        <v>5780</v>
-      </c>
-      <c r="K359" s="2" t="s">
-        <v>5781</v>
-      </c>
-      <c r="L359" s="2" t="s">
-        <v>5782</v>
-      </c>
-      <c r="M359" s="2" t="s">
-        <v>5783</v>
-      </c>
-      <c r="N359" s="2" t="s">
-        <v>5784</v>
-      </c>
-      <c r="O359" s="2" t="s">
-        <v>5785</v>
-      </c>
       <c r="P359" s="2" t="s">
-        <v>5786</v>
-      </c>
-      <c r="R359" s="2" t="s">
-        <v>5787</v>
+        <v>5767</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="2" t="s">
+        <v>5776</v>
+      </c>
+      <c r="C360" s="2" t="s">
+        <v>5777</v>
+      </c>
+      <c r="D360" s="1" t="s">
+        <v>5778</v>
+      </c>
+      <c r="E360" s="2" t="s">
+        <v>5779</v>
+      </c>
+      <c r="F360" s="2" t="s">
+        <v>5780</v>
+      </c>
+      <c r="H360" s="2" t="s">
+        <v>5781</v>
+      </c>
+      <c r="I360" s="2" t="s">
+        <v>5782</v>
+      </c>
+      <c r="J360" s="2" t="s">
+        <v>5783</v>
+      </c>
+      <c r="K360" s="2" t="s">
+        <v>5784</v>
+      </c>
+      <c r="L360" s="2" t="s">
+        <v>5785</v>
+      </c>
+      <c r="M360" s="2" t="s">
+        <v>5786</v>
+      </c>
+      <c r="N360" s="2" t="s">
+        <v>5787</v>
+      </c>
+      <c r="O360" s="2" t="s">
         <v>5788</v>
       </c>
-      <c r="C360" s="2" t="s">
+      <c r="P360" s="2" t="s">
         <v>5789</v>
       </c>
-      <c r="D360" s="1" t="s">
+      <c r="R360" s="2" t="s">
         <v>5790</v>
-      </c>
-      <c r="F360" s="2" t="s">
-        <v>5791</v>
-      </c>
-      <c r="H360" s="2" t="s">
-        <v>5792</v>
-      </c>
-      <c r="I360" s="2" t="s">
-        <v>5793</v>
-      </c>
-      <c r="J360" s="2" t="s">
-        <v>5794</v>
-      </c>
-      <c r="K360" s="2" t="s">
-        <v>5795</v>
-      </c>
-      <c r="L360" s="2" t="s">
-        <v>5796</v>
-      </c>
-      <c r="M360" s="2" t="s">
-        <v>5797</v>
-      </c>
-      <c r="N360" s="2" t="s">
-        <v>5798</v>
-      </c>
-      <c r="O360" s="2" t="s">
-        <v>5799</v>
-      </c>
-      <c r="P360" s="2" t="s">
-        <v>5800</v>
-      </c>
-      <c r="R360" s="2" t="s">
-        <v>5801</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="2" t="s">
+        <v>5791</v>
+      </c>
+      <c r="C361" s="2" t="s">
+        <v>5792</v>
+      </c>
+      <c r="D361" s="1" t="s">
+        <v>5793</v>
+      </c>
+      <c r="F361" s="2" t="s">
+        <v>5794</v>
+      </c>
+      <c r="H361" s="2" t="s">
+        <v>5795</v>
+      </c>
+      <c r="I361" s="2" t="s">
+        <v>5796</v>
+      </c>
+      <c r="J361" s="2" t="s">
+        <v>5797</v>
+      </c>
+      <c r="K361" s="2" t="s">
+        <v>5798</v>
+      </c>
+      <c r="L361" s="2" t="s">
+        <v>5799</v>
+      </c>
+      <c r="M361" s="2" t="s">
+        <v>5800</v>
+      </c>
+      <c r="N361" s="2" t="s">
+        <v>5801</v>
+      </c>
+      <c r="O361" s="2" t="s">
         <v>5802</v>
       </c>
-      <c r="C361" s="2" t="s">
+      <c r="P361" s="2" t="s">
         <v>5803</v>
       </c>
-      <c r="D361" s="1" t="s">
+      <c r="R361" s="2" t="s">
         <v>5804</v>
-      </c>
-      <c r="E361" s="2" t="s">
-        <v>5805</v>
-      </c>
-      <c r="F361" s="2" t="s">
-        <v>5806</v>
-      </c>
-      <c r="G361" s="2" t="s">
-        <v>5807</v>
-      </c>
-      <c r="H361" s="2" t="s">
-        <v>5808</v>
-      </c>
-      <c r="I361" s="2" t="s">
-        <v>5809</v>
-      </c>
-      <c r="J361" s="2" t="s">
-        <v>5810</v>
-      </c>
-      <c r="K361" s="2" t="s">
-        <v>5811</v>
-      </c>
-      <c r="L361" s="2" t="s">
-        <v>5812</v>
-      </c>
-      <c r="M361" s="2" t="s">
-        <v>5813</v>
-      </c>
-      <c r="N361" s="2" t="s">
-        <v>5814</v>
-      </c>
-      <c r="O361" s="2" t="s">
-        <v>5815</v>
-      </c>
-      <c r="P361" s="2" t="s">
-        <v>5816</v>
-      </c>
-      <c r="R361" s="2" t="s">
-        <v>5817</v>
-      </c>
-      <c r="T361" s="2" t="s">
-        <v>5818</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="2" t="s">
+        <v>5805</v>
+      </c>
+      <c r="C362" s="2" t="s">
+        <v>5806</v>
+      </c>
+      <c r="D362" s="1" t="s">
+        <v>5807</v>
+      </c>
+      <c r="E362" s="2" t="s">
+        <v>5808</v>
+      </c>
+      <c r="F362" s="2" t="s">
+        <v>5809</v>
+      </c>
+      <c r="G362" s="2" t="s">
+        <v>5810</v>
+      </c>
+      <c r="H362" s="2" t="s">
+        <v>5811</v>
+      </c>
+      <c r="I362" s="2" t="s">
+        <v>5812</v>
+      </c>
+      <c r="J362" s="2" t="s">
+        <v>5813</v>
+      </c>
+      <c r="K362" s="2" t="s">
+        <v>5814</v>
+      </c>
+      <c r="L362" s="2" t="s">
+        <v>5815</v>
+      </c>
+      <c r="M362" s="2" t="s">
+        <v>5816</v>
+      </c>
+      <c r="N362" s="2" t="s">
+        <v>5817</v>
+      </c>
+      <c r="O362" s="2" t="s">
+        <v>5818</v>
+      </c>
+      <c r="P362" s="2" t="s">
         <v>5819</v>
       </c>
-      <c r="C362" s="2" t="s">
+      <c r="R362" s="2" t="s">
         <v>5820</v>
       </c>
-      <c r="D362" s="1" t="s">
+      <c r="T362" s="2" t="s">
         <v>5821</v>
-      </c>
-      <c r="F362" s="2" t="s">
-        <v>5822</v>
-      </c>
-      <c r="G362" s="2" t="s">
-        <v>5823</v>
-      </c>
-      <c r="H362" s="2" t="s">
-        <v>5824</v>
-      </c>
-      <c r="I362" s="2" t="s">
-        <v>5820</v>
-      </c>
-      <c r="J362" s="2" t="s">
-        <v>5825</v>
-      </c>
-      <c r="K362" s="2" t="s">
-        <v>5826</v>
-      </c>
-      <c r="L362" s="2" t="s">
-        <v>5827</v>
-      </c>
-      <c r="M362" s="2" t="s">
-        <v>5828</v>
-      </c>
-      <c r="N362" s="2" t="s">
-        <v>5829</v>
-      </c>
-      <c r="O362" s="2" t="s">
-        <v>5830</v>
-      </c>
-      <c r="P362" s="2" t="s">
-        <v>5820</v>
-      </c>
-      <c r="T362" s="2" t="s">
-        <v>5831</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="2" t="s">
+        <v>5822</v>
+      </c>
+      <c r="C363" s="2" t="s">
+        <v>5823</v>
+      </c>
+      <c r="D363" s="1" t="s">
+        <v>5824</v>
+      </c>
+      <c r="F363" s="2" t="s">
+        <v>5825</v>
+      </c>
+      <c r="G363" s="2" t="s">
+        <v>5826</v>
+      </c>
+      <c r="H363" s="2" t="s">
+        <v>5827</v>
+      </c>
+      <c r="I363" s="2" t="s">
+        <v>5823</v>
+      </c>
+      <c r="J363" s="2" t="s">
+        <v>5828</v>
+      </c>
+      <c r="K363" s="2" t="s">
+        <v>5829</v>
+      </c>
+      <c r="L363" s="2" t="s">
+        <v>5830</v>
+      </c>
+      <c r="M363" s="2" t="s">
+        <v>5831</v>
+      </c>
+      <c r="N363" s="2" t="s">
         <v>5832</v>
       </c>
-      <c r="C363" s="2" t="s">
+      <c r="O363" s="2" t="s">
         <v>5833</v>
       </c>
-      <c r="D363" s="2" t="s">
+      <c r="P363" s="2" t="s">
+        <v>5823</v>
+      </c>
+      <c r="T363" s="2" t="s">
         <v>5834</v>
-      </c>
-      <c r="E363" s="2" t="s">
-        <v>5835</v>
-      </c>
-      <c r="G363" s="2" t="s">
-        <v>5836</v>
-      </c>
-      <c r="H363" s="2" t="s">
-        <v>5835</v>
-      </c>
-      <c r="I363" s="2" t="s">
-        <v>5837</v>
-      </c>
-      <c r="J363" s="2" t="s">
-        <v>5838</v>
-      </c>
-      <c r="K363" s="2" t="s">
-        <v>5839</v>
-      </c>
-      <c r="L363" s="2" t="s">
-        <v>5835</v>
-      </c>
-      <c r="M363" s="2" t="s">
-        <v>5840</v>
-      </c>
-      <c r="O363" s="2" t="s">
-        <v>5841</v>
-      </c>
-      <c r="P363" s="2" t="s">
-        <v>5842</v>
-      </c>
-      <c r="Q363" s="2" t="s">
-        <v>5843</v>
-      </c>
-      <c r="R363" s="2" t="s">
-        <v>5844</v>
-      </c>
-      <c r="S363" s="2" t="s">
-        <v>5845</v>
-      </c>
-      <c r="T363" s="2" t="s">
-        <v>5835</v>
-      </c>
-      <c r="U363" s="2" t="s">
-        <v>5833</v>
-      </c>
-      <c r="V363" s="2" t="s">
-        <v>5846</v>
-      </c>
-      <c r="W363" s="3" t="s">
-        <v>5847</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="2" t="s">
+        <v>5835</v>
+      </c>
+      <c r="C364" s="2" t="s">
+        <v>5836</v>
+      </c>
+      <c r="D364" s="2" t="s">
+        <v>5837</v>
+      </c>
+      <c r="E364" s="2" t="s">
+        <v>5838</v>
+      </c>
+      <c r="G364" s="2" t="s">
+        <v>5839</v>
+      </c>
+      <c r="H364" s="2" t="s">
+        <v>5838</v>
+      </c>
+      <c r="I364" s="2" t="s">
+        <v>5840</v>
+      </c>
+      <c r="J364" s="2" t="s">
+        <v>5841</v>
+      </c>
+      <c r="K364" s="2" t="s">
+        <v>5842</v>
+      </c>
+      <c r="L364" s="2" t="s">
+        <v>5838</v>
+      </c>
+      <c r="M364" s="2" t="s">
+        <v>5843</v>
+      </c>
+      <c r="O364" s="2" t="s">
+        <v>5844</v>
+      </c>
+      <c r="P364" s="2" t="s">
+        <v>5845</v>
+      </c>
+      <c r="Q364" s="2" t="s">
+        <v>5846</v>
+      </c>
+      <c r="R364" s="2" t="s">
+        <v>5847</v>
+      </c>
+      <c r="S364" s="2" t="s">
         <v>5848</v>
       </c>
-      <c r="C364" s="2" t="s">
+      <c r="T364" s="2" t="s">
+        <v>5838</v>
+      </c>
+      <c r="U364" s="2" t="s">
+        <v>5836</v>
+      </c>
+      <c r="V364" s="2" t="s">
         <v>5849</v>
       </c>
-      <c r="D364" s="2" t="s">
+      <c r="W364" s="3" t="s">
         <v>5850</v>
-      </c>
-      <c r="E364" s="2" t="s">
-        <v>5851</v>
-      </c>
-      <c r="F364" s="2" t="s">
-        <v>5852</v>
-      </c>
-      <c r="G364" s="2" t="s">
-        <v>5853</v>
-      </c>
-      <c r="H364" s="2" t="s">
-        <v>5854</v>
-      </c>
-      <c r="I364" s="2" t="s">
-        <v>5855</v>
-      </c>
-      <c r="J364" s="2" t="s">
-        <v>5856</v>
-      </c>
-      <c r="K364" s="2" t="s">
-        <v>5857</v>
-      </c>
-      <c r="L364" s="2" t="s">
-        <v>5858</v>
-      </c>
-      <c r="M364" s="2" t="s">
-        <v>5859</v>
-      </c>
-      <c r="O364" s="2" t="s">
-        <v>5851</v>
-      </c>
-      <c r="P364" s="2" t="s">
-        <v>5860</v>
-      </c>
-      <c r="Q364" s="2" t="s">
-        <v>5853</v>
-      </c>
-      <c r="R364" s="2" t="s">
-        <v>5861</v>
-      </c>
-      <c r="S364" s="2" t="s">
-        <v>5862</v>
-      </c>
-      <c r="T364" s="2" t="s">
-        <v>5863</v>
-      </c>
-      <c r="U364" s="2" t="s">
-        <v>5864</v>
-      </c>
-      <c r="V364" s="2" t="s">
-        <v>5865</v>
-      </c>
-      <c r="W364" s="3" t="s">
-        <v>4630</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="2" t="s">
+        <v>5851</v>
+      </c>
+      <c r="C365" s="2" t="s">
+        <v>5852</v>
+      </c>
+      <c r="D365" s="2" t="s">
+        <v>5853</v>
+      </c>
+      <c r="E365" s="2" t="s">
+        <v>5854</v>
+      </c>
+      <c r="F365" s="2" t="s">
+        <v>5855</v>
+      </c>
+      <c r="G365" s="2" t="s">
+        <v>5856</v>
+      </c>
+      <c r="H365" s="2" t="s">
+        <v>5857</v>
+      </c>
+      <c r="I365" s="2" t="s">
+        <v>5858</v>
+      </c>
+      <c r="J365" s="2" t="s">
+        <v>5859</v>
+      </c>
+      <c r="K365" s="2" t="s">
+        <v>5860</v>
+      </c>
+      <c r="L365" s="2" t="s">
+        <v>5861</v>
+      </c>
+      <c r="M365" s="2" t="s">
+        <v>5862</v>
+      </c>
+      <c r="O365" s="2" t="s">
+        <v>5854</v>
+      </c>
+      <c r="P365" s="2" t="s">
+        <v>5863</v>
+      </c>
+      <c r="Q365" s="2" t="s">
+        <v>5856</v>
+      </c>
+      <c r="R365" s="2" t="s">
+        <v>5864</v>
+      </c>
+      <c r="S365" s="2" t="s">
+        <v>5865</v>
+      </c>
+      <c r="T365" s="2" t="s">
         <v>5866</v>
       </c>
-      <c r="C365" s="2" t="s">
+      <c r="U365" s="2" t="s">
         <v>5867</v>
       </c>
-      <c r="D365" s="1" t="s">
+      <c r="V365" s="2" t="s">
         <v>5868</v>
       </c>
-      <c r="E365" s="2" t="s">
-        <v>5869</v>
-      </c>
-      <c r="F365" s="2" t="s">
-        <v>5870</v>
-      </c>
-      <c r="G365" s="2" t="s">
-        <v>5871</v>
-      </c>
-      <c r="H365" s="2" t="s">
-        <v>5872</v>
-      </c>
-      <c r="I365" s="2" t="s">
-        <v>5873</v>
-      </c>
-      <c r="J365" s="2" t="s">
-        <v>5874</v>
-      </c>
-      <c r="K365" s="2" t="s">
-        <v>5875</v>
-      </c>
-      <c r="L365" s="2" t="s">
-        <v>5876</v>
-      </c>
-      <c r="M365" s="2" t="s">
-        <v>5877</v>
-      </c>
-      <c r="N365" s="2" t="s">
-        <v>5878</v>
-      </c>
-      <c r="O365" s="2" t="s">
-        <v>5879</v>
-      </c>
-      <c r="P365" s="2" t="s">
-        <v>5880</v>
-      </c>
-      <c r="R365" s="2" t="s">
-        <v>5881</v>
-      </c>
-      <c r="T365" s="2" t="s">
-        <v>5882</v>
+      <c r="W365" s="3" t="s">
+        <v>4630</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="2" t="s">
+        <v>5869</v>
+      </c>
+      <c r="C366" s="2" t="s">
+        <v>5870</v>
+      </c>
+      <c r="D366" s="1" t="s">
+        <v>5871</v>
+      </c>
+      <c r="E366" s="2" t="s">
+        <v>5872</v>
+      </c>
+      <c r="F366" s="2" t="s">
+        <v>5873</v>
+      </c>
+      <c r="G366" s="2" t="s">
+        <v>5874</v>
+      </c>
+      <c r="H366" s="2" t="s">
+        <v>5875</v>
+      </c>
+      <c r="I366" s="2" t="s">
+        <v>5876</v>
+      </c>
+      <c r="J366" s="2" t="s">
+        <v>5877</v>
+      </c>
+      <c r="K366" s="2" t="s">
+        <v>5878</v>
+      </c>
+      <c r="L366" s="2" t="s">
+        <v>5879</v>
+      </c>
+      <c r="M366" s="2" t="s">
+        <v>5880</v>
+      </c>
+      <c r="N366" s="2" t="s">
+        <v>5881</v>
+      </c>
+      <c r="O366" s="2" t="s">
+        <v>5882</v>
+      </c>
+      <c r="P366" s="2" t="s">
         <v>5883</v>
       </c>
-      <c r="C366" s="2" t="s">
+      <c r="R366" s="2" t="s">
         <v>5884</v>
       </c>
-      <c r="D366" s="1" t="s">
+      <c r="T366" s="2" t="s">
         <v>5885</v>
-      </c>
-      <c r="E366" s="2" t="s">
-        <v>5886</v>
-      </c>
-      <c r="F366" s="2" t="s">
-        <v>5887</v>
-      </c>
-      <c r="G366" s="2" t="s">
-        <v>5888</v>
-      </c>
-      <c r="H366" s="2" t="s">
-        <v>5889</v>
-      </c>
-      <c r="I366" s="2" t="s">
-        <v>5890</v>
-      </c>
-      <c r="J366" s="2" t="s">
-        <v>2932</v>
-      </c>
-      <c r="K366" s="2" t="s">
-        <v>5891</v>
-      </c>
-      <c r="L366" s="2" t="s">
-        <v>5892</v>
-      </c>
-      <c r="M366" s="2" t="s">
-        <v>5893</v>
-      </c>
-      <c r="N366" s="2" t="s">
-        <v>5894</v>
-      </c>
-      <c r="O366" s="2" t="s">
-        <v>5886</v>
-      </c>
-      <c r="P366" s="2" t="s">
-        <v>5895</v>
-      </c>
-      <c r="R366" s="2" t="s">
-        <v>5896</v>
-      </c>
-      <c r="T366" s="2" t="s">
-        <v>5897</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="2" t="s">
+        <v>5886</v>
+      </c>
+      <c r="C367" s="2" t="s">
+        <v>5887</v>
+      </c>
+      <c r="D367" s="1" t="s">
+        <v>5888</v>
+      </c>
+      <c r="E367" s="2" t="s">
+        <v>5889</v>
+      </c>
+      <c r="F367" s="2" t="s">
+        <v>5890</v>
+      </c>
+      <c r="G367" s="2" t="s">
+        <v>5891</v>
+      </c>
+      <c r="H367" s="2" t="s">
+        <v>5892</v>
+      </c>
+      <c r="I367" s="2" t="s">
+        <v>5893</v>
+      </c>
+      <c r="J367" s="2" t="s">
+        <v>2932</v>
+      </c>
+      <c r="K367" s="2" t="s">
+        <v>5894</v>
+      </c>
+      <c r="L367" s="2" t="s">
+        <v>5895</v>
+      </c>
+      <c r="M367" s="2" t="s">
+        <v>5896</v>
+      </c>
+      <c r="N367" s="2" t="s">
+        <v>5897</v>
+      </c>
+      <c r="O367" s="2" t="s">
+        <v>5889</v>
+      </c>
+      <c r="P367" s="2" t="s">
         <v>5898</v>
       </c>
-      <c r="C367" s="2" t="s">
+      <c r="R367" s="2" t="s">
         <v>5899</v>
       </c>
-      <c r="D367" s="2" t="s">
+      <c r="T367" s="2" t="s">
         <v>5900</v>
-      </c>
-      <c r="E367" s="2" t="s">
-        <v>5901</v>
-      </c>
-      <c r="F367" s="2" t="s">
-        <v>5902</v>
-      </c>
-      <c r="G367" s="2" t="s">
-        <v>5903</v>
-      </c>
-      <c r="H367" s="2" t="s">
-        <v>5904</v>
-      </c>
-      <c r="I367" s="2" t="s">
-        <v>5905</v>
-      </c>
-      <c r="J367" s="2" t="s">
-        <v>5906</v>
-      </c>
-      <c r="K367" s="2" t="s">
-        <v>5907</v>
-      </c>
-      <c r="L367" s="2" t="s">
-        <v>5908</v>
-      </c>
-      <c r="M367" s="2" t="s">
-        <v>5909</v>
-      </c>
-      <c r="N367" s="2" t="s">
-        <v>5910</v>
-      </c>
-      <c r="O367" s="2" t="s">
-        <v>5911</v>
-      </c>
-      <c r="P367" s="2" t="s">
-        <v>5912</v>
-      </c>
-      <c r="Q367" s="2" t="s">
-        <v>5913</v>
-      </c>
-      <c r="R367" s="2" t="s">
-        <v>5914</v>
-      </c>
-      <c r="T367" s="2" t="s">
-        <v>5915</v>
-      </c>
-      <c r="V367" s="2" t="s">
-        <v>5916</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="2" t="s">
+        <v>5901</v>
+      </c>
+      <c r="C368" s="2" t="s">
+        <v>5902</v>
+      </c>
+      <c r="D368" s="2" t="s">
+        <v>5903</v>
+      </c>
+      <c r="E368" s="2" t="s">
+        <v>5904</v>
+      </c>
+      <c r="F368" s="2" t="s">
+        <v>5905</v>
+      </c>
+      <c r="G368" s="2" t="s">
+        <v>5906</v>
+      </c>
+      <c r="H368" s="2" t="s">
+        <v>5907</v>
+      </c>
+      <c r="I368" s="2" t="s">
+        <v>5908</v>
+      </c>
+      <c r="J368" s="2" t="s">
+        <v>5909</v>
+      </c>
+      <c r="K368" s="2" t="s">
+        <v>5910</v>
+      </c>
+      <c r="L368" s="2" t="s">
+        <v>5911</v>
+      </c>
+      <c r="M368" s="2" t="s">
+        <v>5912</v>
+      </c>
+      <c r="N368" s="2" t="s">
+        <v>5913</v>
+      </c>
+      <c r="O368" s="2" t="s">
+        <v>5914</v>
+      </c>
+      <c r="P368" s="2" t="s">
+        <v>5915</v>
+      </c>
+      <c r="Q368" s="2" t="s">
+        <v>5916</v>
+      </c>
+      <c r="R368" s="2" t="s">
         <v>5917</v>
       </c>
-      <c r="C368" s="2" t="s">
+      <c r="T368" s="2" t="s">
         <v>5918</v>
       </c>
-      <c r="D368" s="1" t="s">
+      <c r="V368" s="2" t="s">
         <v>5919</v>
-      </c>
-      <c r="F368" s="2" t="s">
-        <v>5920</v>
-      </c>
-      <c r="G368" s="2" t="s">
-        <v>5921</v>
-      </c>
-      <c r="H368" s="2" t="s">
-        <v>5922</v>
-      </c>
-      <c r="I368" s="2" t="s">
-        <v>5923</v>
-      </c>
-      <c r="J368" s="2" t="s">
-        <v>5924</v>
-      </c>
-      <c r="K368" s="2" t="s">
-        <v>5925</v>
-      </c>
-      <c r="L368" s="2" t="s">
-        <v>5926</v>
-      </c>
-      <c r="M368" s="2" t="s">
-        <v>5927</v>
-      </c>
-      <c r="O368" s="2" t="s">
-        <v>5928</v>
-      </c>
-      <c r="P368" s="2" t="s">
-        <v>5918</v>
-      </c>
-      <c r="T368" s="2" t="s">
-        <v>5929</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="2" t="s">
+        <v>5920</v>
+      </c>
+      <c r="C369" s="2" t="s">
+        <v>5921</v>
+      </c>
+      <c r="D369" s="1" t="s">
+        <v>5922</v>
+      </c>
+      <c r="F369" s="2" t="s">
+        <v>5923</v>
+      </c>
+      <c r="G369" s="2" t="s">
+        <v>5924</v>
+      </c>
+      <c r="H369" s="2" t="s">
+        <v>5925</v>
+      </c>
+      <c r="I369" s="2" t="s">
+        <v>5926</v>
+      </c>
+      <c r="J369" s="2" t="s">
+        <v>5927</v>
+      </c>
+      <c r="K369" s="2" t="s">
+        <v>5928</v>
+      </c>
+      <c r="L369" s="2" t="s">
+        <v>5929</v>
+      </c>
+      <c r="M369" s="2" t="s">
         <v>5930</v>
       </c>
-      <c r="C369" s="2" t="s">
+      <c r="O369" s="2" t="s">
         <v>5931</v>
       </c>
-      <c r="D369" s="2" t="s">
+      <c r="P369" s="2" t="s">
+        <v>5921</v>
+      </c>
+      <c r="T369" s="2" t="s">
         <v>5932</v>
-      </c>
-      <c r="F369" s="2" t="s">
-        <v>5933</v>
-      </c>
-      <c r="G369" s="2" t="s">
-        <v>5934</v>
-      </c>
-      <c r="H369" s="2" t="s">
-        <v>5935</v>
-      </c>
-      <c r="I369" s="2" t="s">
-        <v>5936</v>
-      </c>
-      <c r="J369" s="2" t="s">
-        <v>5937</v>
-      </c>
-      <c r="K369" s="2" t="s">
-        <v>5938</v>
-      </c>
-      <c r="L369" s="2" t="s">
-        <v>5939</v>
-      </c>
-      <c r="M369" s="2" t="s">
-        <v>5940</v>
-      </c>
-      <c r="O369" s="2" t="s">
-        <v>5941</v>
-      </c>
-      <c r="P369" s="2" t="s">
-        <v>5942</v>
-      </c>
-      <c r="Q369" s="2" t="s">
-        <v>5943</v>
-      </c>
-      <c r="R369" s="2" t="s">
-        <v>5944</v>
-      </c>
-      <c r="S369" s="2" t="s">
-        <v>5945</v>
-      </c>
-      <c r="T369" s="2" t="s">
-        <v>5946</v>
-      </c>
-      <c r="V369" s="2" t="s">
-        <v>5947</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="2" t="s">
+        <v>5933</v>
+      </c>
+      <c r="C370" s="2" t="s">
+        <v>5934</v>
+      </c>
+      <c r="D370" s="2" t="s">
+        <v>5935</v>
+      </c>
+      <c r="F370" s="2" t="s">
+        <v>5936</v>
+      </c>
+      <c r="G370" s="2" t="s">
+        <v>5937</v>
+      </c>
+      <c r="H370" s="2" t="s">
+        <v>5938</v>
+      </c>
+      <c r="I370" s="2" t="s">
+        <v>5939</v>
+      </c>
+      <c r="J370" s="2" t="s">
+        <v>5940</v>
+      </c>
+      <c r="K370" s="2" t="s">
+        <v>5941</v>
+      </c>
+      <c r="L370" s="2" t="s">
+        <v>5942</v>
+      </c>
+      <c r="M370" s="2" t="s">
+        <v>5943</v>
+      </c>
+      <c r="O370" s="2" t="s">
+        <v>5944</v>
+      </c>
+      <c r="P370" s="2" t="s">
+        <v>5945</v>
+      </c>
+      <c r="Q370" s="2" t="s">
+        <v>5946</v>
+      </c>
+      <c r="R370" s="2" t="s">
+        <v>5947</v>
+      </c>
+      <c r="S370" s="2" t="s">
         <v>5948</v>
       </c>
-      <c r="C370" s="2" t="s">
+      <c r="T370" s="2" t="s">
         <v>5949</v>
       </c>
-      <c r="D370" s="1" t="s">
+      <c r="V370" s="2" t="s">
         <v>5950</v>
-      </c>
-      <c r="E370" s="2" t="s">
-        <v>5951</v>
-      </c>
-      <c r="F370" s="2" t="s">
-        <v>5952</v>
-      </c>
-      <c r="G370" s="2" t="s">
-        <v>5953</v>
-      </c>
-      <c r="H370" s="2" t="s">
-        <v>5954</v>
-      </c>
-      <c r="I370" s="2" t="s">
-        <v>5955</v>
-      </c>
-      <c r="J370" s="2" t="s">
-        <v>5956</v>
-      </c>
-      <c r="K370" s="2" t="s">
-        <v>5957</v>
-      </c>
-      <c r="L370" s="2" t="s">
-        <v>5958</v>
-      </c>
-      <c r="M370" s="2" t="s">
-        <v>5959</v>
-      </c>
-      <c r="N370" s="2" t="s">
-        <v>5960</v>
-      </c>
-      <c r="O370" s="2" t="s">
-        <v>5961</v>
-      </c>
-      <c r="P370" s="2" t="s">
-        <v>5949</v>
-      </c>
-      <c r="R370" s="2" t="s">
-        <v>5962</v>
-      </c>
-      <c r="T370" s="2" t="s">
-        <v>5963</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="2" t="s">
+        <v>5951</v>
+      </c>
+      <c r="C371" s="2" t="s">
+        <v>5952</v>
+      </c>
+      <c r="D371" s="1" t="s">
+        <v>5953</v>
+      </c>
+      <c r="E371" s="2" t="s">
+        <v>5954</v>
+      </c>
+      <c r="F371" s="2" t="s">
+        <v>5955</v>
+      </c>
+      <c r="G371" s="2" t="s">
+        <v>5956</v>
+      </c>
+      <c r="H371" s="2" t="s">
+        <v>5957</v>
+      </c>
+      <c r="I371" s="2" t="s">
+        <v>5958</v>
+      </c>
+      <c r="J371" s="2" t="s">
+        <v>5959</v>
+      </c>
+      <c r="K371" s="2" t="s">
+        <v>5960</v>
+      </c>
+      <c r="L371" s="2" t="s">
+        <v>5961</v>
+      </c>
+      <c r="M371" s="2" t="s">
+        <v>5962</v>
+      </c>
+      <c r="N371" s="2" t="s">
+        <v>5963</v>
+      </c>
+      <c r="O371" s="2" t="s">
         <v>5964</v>
       </c>
-      <c r="C371" s="2" t="s">
+      <c r="P371" s="2" t="s">
+        <v>5952</v>
+      </c>
+      <c r="R371" s="2" t="s">
         <v>5965</v>
       </c>
-      <c r="D371" s="1" t="s">
+      <c r="T371" s="2" t="s">
         <v>5966</v>
-      </c>
-      <c r="E371" s="2" t="s">
-        <v>5967</v>
-      </c>
-      <c r="F371" s="2" t="s">
-        <v>5968</v>
-      </c>
-      <c r="G371" s="2" t="s">
-        <v>5969</v>
-      </c>
-      <c r="H371" s="2" t="s">
-        <v>5970</v>
-      </c>
-      <c r="I371" s="2" t="s">
-        <v>5971</v>
-      </c>
-      <c r="J371" s="2" t="s">
-        <v>2932</v>
-      </c>
-      <c r="K371" s="2" t="s">
-        <v>5891</v>
-      </c>
-      <c r="L371" s="2" t="s">
-        <v>5972</v>
-      </c>
-      <c r="M371" s="2" t="s">
-        <v>5973</v>
-      </c>
-      <c r="N371" s="2" t="s">
-        <v>5974</v>
-      </c>
-      <c r="O371" s="2" t="s">
-        <v>5975</v>
-      </c>
-      <c r="P371" s="2" t="s">
-        <v>5965</v>
-      </c>
-      <c r="R371" s="2" t="s">
-        <v>5976</v>
-      </c>
-      <c r="T371" s="2" t="s">
-        <v>5977</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="2" t="s">
+        <v>5967</v>
+      </c>
+      <c r="C372" s="2" t="s">
+        <v>5968</v>
+      </c>
+      <c r="D372" s="1" t="s">
+        <v>5969</v>
+      </c>
+      <c r="E372" s="2" t="s">
+        <v>5970</v>
+      </c>
+      <c r="F372" s="2" t="s">
+        <v>5971</v>
+      </c>
+      <c r="G372" s="2" t="s">
+        <v>5972</v>
+      </c>
+      <c r="H372" s="2" t="s">
+        <v>5973</v>
+      </c>
+      <c r="I372" s="2" t="s">
+        <v>5974</v>
+      </c>
+      <c r="J372" s="2" t="s">
+        <v>2932</v>
+      </c>
+      <c r="K372" s="2" t="s">
+        <v>5894</v>
+      </c>
+      <c r="L372" s="2" t="s">
+        <v>5975</v>
+      </c>
+      <c r="M372" s="2" t="s">
+        <v>5976</v>
+      </c>
+      <c r="N372" s="2" t="s">
+        <v>5977</v>
+      </c>
+      <c r="O372" s="2" t="s">
         <v>5978</v>
       </c>
-      <c r="C372" s="2" t="s">
+      <c r="P372" s="2" t="s">
+        <v>5968</v>
+      </c>
+      <c r="R372" s="2" t="s">
         <v>5979</v>
       </c>
-      <c r="D372" s="1" t="s">
+      <c r="T372" s="2" t="s">
         <v>5980</v>
-      </c>
-      <c r="E372" s="2" t="s">
-        <v>5981</v>
-      </c>
-      <c r="F372" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="G372" s="2" t="s">
-        <v>5982</v>
-      </c>
-      <c r="H372" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="I372" s="2" t="s">
-        <v>5983</v>
-      </c>
-      <c r="J372" s="2" t="s">
-        <v>5984</v>
-      </c>
-      <c r="K372" s="2" t="s">
-        <v>5985</v>
-      </c>
-      <c r="L372" s="2" t="s">
-        <v>5986</v>
-      </c>
-      <c r="M372" s="2" t="s">
-        <v>5987</v>
-      </c>
-      <c r="N372" s="2" t="s">
-        <v>5988</v>
-      </c>
-      <c r="O372" s="2" t="s">
-        <v>5989</v>
-      </c>
-      <c r="P372" s="2" t="s">
-        <v>5979</v>
-      </c>
-      <c r="T372" s="2" t="s">
-        <v>5990</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="2" t="s">
+        <v>5981</v>
+      </c>
+      <c r="C373" s="2" t="s">
+        <v>5982</v>
+      </c>
+      <c r="D373" s="1" t="s">
+        <v>5983</v>
+      </c>
+      <c r="E373" s="2" t="s">
+        <v>5984</v>
+      </c>
+      <c r="F373" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G373" s="2" t="s">
+        <v>5985</v>
+      </c>
+      <c r="H373" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="I373" s="2" t="s">
+        <v>5986</v>
+      </c>
+      <c r="J373" s="2" t="s">
+        <v>5987</v>
+      </c>
+      <c r="K373" s="2" t="s">
+        <v>5988</v>
+      </c>
+      <c r="L373" s="2" t="s">
+        <v>5989</v>
+      </c>
+      <c r="M373" s="2" t="s">
+        <v>5990</v>
+      </c>
+      <c r="N373" s="2" t="s">
         <v>5991</v>
       </c>
-      <c r="C373" s="2" t="s">
+      <c r="O373" s="2" t="s">
         <v>5992</v>
       </c>
-      <c r="D373" s="2" t="s">
+      <c r="P373" s="2" t="s">
+        <v>5982</v>
+      </c>
+      <c r="T373" s="2" t="s">
         <v>5993</v>
-      </c>
-      <c r="F373" s="2" t="s">
-        <v>5994</v>
-      </c>
-      <c r="G373" s="2" t="s">
-        <v>5995</v>
-      </c>
-      <c r="H373" s="2" t="s">
-        <v>5996</v>
-      </c>
-      <c r="I373" s="2" t="s">
-        <v>5997</v>
-      </c>
-      <c r="J373" s="2" t="s">
-        <v>5998</v>
-      </c>
-      <c r="K373" s="2" t="s">
-        <v>5999</v>
-      </c>
-      <c r="L373" s="2" t="s">
-        <v>6000</v>
-      </c>
-      <c r="M373" s="2" t="s">
-        <v>6001</v>
-      </c>
-      <c r="N373" s="2" t="s">
-        <v>6002</v>
-      </c>
-      <c r="O373" s="2" t="s">
-        <v>6003</v>
-      </c>
-      <c r="P373" s="2" t="s">
-        <v>6004</v>
-      </c>
-      <c r="Q373" s="2" t="s">
-        <v>5995</v>
-      </c>
-      <c r="R373" s="2" t="s">
-        <v>6005</v>
-      </c>
-      <c r="S373" s="2" t="s">
-        <v>6006</v>
-      </c>
-      <c r="V373" s="2" t="s">
-        <v>6007</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="2" t="s">
+        <v>5994</v>
+      </c>
+      <c r="C374" s="2" t="s">
+        <v>5995</v>
+      </c>
+      <c r="D374" s="2" t="s">
+        <v>5996</v>
+      </c>
+      <c r="F374" s="2" t="s">
+        <v>5997</v>
+      </c>
+      <c r="G374" s="2" t="s">
+        <v>5998</v>
+      </c>
+      <c r="H374" s="2" t="s">
+        <v>5999</v>
+      </c>
+      <c r="I374" s="2" t="s">
+        <v>6000</v>
+      </c>
+      <c r="J374" s="2" t="s">
+        <v>6001</v>
+      </c>
+      <c r="K374" s="2" t="s">
+        <v>6002</v>
+      </c>
+      <c r="L374" s="2" t="s">
+        <v>6003</v>
+      </c>
+      <c r="M374" s="2" t="s">
+        <v>6004</v>
+      </c>
+      <c r="N374" s="2" t="s">
+        <v>6005</v>
+      </c>
+      <c r="O374" s="2" t="s">
+        <v>6006</v>
+      </c>
+      <c r="P374" s="2" t="s">
+        <v>6007</v>
+      </c>
+      <c r="Q374" s="2" t="s">
+        <v>5998</v>
+      </c>
+      <c r="R374" s="2" t="s">
         <v>6008</v>
       </c>
-      <c r="C374" s="2" t="s">
+      <c r="S374" s="2" t="s">
         <v>6009</v>
       </c>
-      <c r="D374" s="1" t="s">
+      <c r="V374" s="2" t="s">
         <v>6010</v>
-      </c>
-      <c r="F374" s="2" t="s">
-        <v>6011</v>
-      </c>
-      <c r="G374" s="2" t="s">
-        <v>6012</v>
-      </c>
-      <c r="H374" s="2" t="s">
-        <v>6013</v>
-      </c>
-      <c r="I374" s="2" t="s">
-        <v>6014</v>
-      </c>
-      <c r="J374" s="2" t="s">
-        <v>6015</v>
-      </c>
-      <c r="K374" s="2" t="s">
-        <v>6016</v>
-      </c>
-      <c r="L374" s="2" t="s">
-        <v>6017</v>
-      </c>
-      <c r="M374" s="2" t="s">
-        <v>6018</v>
-      </c>
-      <c r="N374" s="2" t="s">
-        <v>6019</v>
-      </c>
-      <c r="O374" s="2" t="s">
-        <v>6020</v>
-      </c>
-      <c r="P374" s="2" t="s">
-        <v>6009</v>
-      </c>
-      <c r="R374" s="2" t="s">
-        <v>6021</v>
-      </c>
-      <c r="T374" s="2" t="s">
-        <v>6022</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="2" t="s">
+        <v>6011</v>
+      </c>
+      <c r="C375" s="2" t="s">
+        <v>6012</v>
+      </c>
+      <c r="D375" s="1" t="s">
+        <v>6013</v>
+      </c>
+      <c r="F375" s="2" t="s">
+        <v>6014</v>
+      </c>
+      <c r="G375" s="2" t="s">
+        <v>6015</v>
+      </c>
+      <c r="H375" s="2" t="s">
+        <v>6016</v>
+      </c>
+      <c r="I375" s="2" t="s">
+        <v>6017</v>
+      </c>
+      <c r="J375" s="2" t="s">
+        <v>6018</v>
+      </c>
+      <c r="K375" s="2" t="s">
+        <v>6019</v>
+      </c>
+      <c r="L375" s="2" t="s">
+        <v>6020</v>
+      </c>
+      <c r="M375" s="2" t="s">
+        <v>6021</v>
+      </c>
+      <c r="N375" s="2" t="s">
+        <v>6022</v>
+      </c>
+      <c r="O375" s="2" t="s">
         <v>6023</v>
       </c>
-      <c r="C375" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="D375" s="1" t="s">
+      <c r="P375" s="2" t="s">
+        <v>6012</v>
+      </c>
+      <c r="R375" s="2" t="s">
         <v>6024</v>
       </c>
-      <c r="G375" s="2" t="s">
+      <c r="T375" s="2" t="s">
         <v>6025</v>
-      </c>
-      <c r="H375" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="I375" s="2" t="s">
-        <v>6026</v>
-      </c>
-      <c r="J375" s="2" t="s">
-        <v>6027</v>
-      </c>
-      <c r="K375" s="2" t="s">
-        <v>6028</v>
-      </c>
-      <c r="L375" s="2" t="s">
-        <v>6028</v>
-      </c>
-      <c r="M375" s="2" t="s">
-        <v>6028</v>
-      </c>
-      <c r="O375" s="2" t="s">
-        <v>6029</v>
-      </c>
-      <c r="P375" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="R375" s="2" t="s">
-        <v>6030</v>
-      </c>
-      <c r="T375" s="2" t="s">
-        <v>6028</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="2" t="s">
+        <v>6026</v>
+      </c>
+      <c r="C376" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="D376" s="1" t="s">
+        <v>6027</v>
+      </c>
+      <c r="G376" s="2" t="s">
+        <v>6028</v>
+      </c>
+      <c r="H376" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="I376" s="2" t="s">
+        <v>6029</v>
+      </c>
+      <c r="J376" s="2" t="s">
+        <v>6030</v>
+      </c>
+      <c r="K376" s="2" t="s">
         <v>6031</v>
       </c>
-      <c r="C376" s="2" t="s">
+      <c r="L376" s="2" t="s">
+        <v>6031</v>
+      </c>
+      <c r="M376" s="2" t="s">
+        <v>6031</v>
+      </c>
+      <c r="O376" s="2" t="s">
         <v>6032</v>
       </c>
-      <c r="D376" s="1" t="s">
+      <c r="P376" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="R376" s="2" t="s">
         <v>6033</v>
       </c>
-      <c r="G376" s="2" t="s">
-        <v>6034</v>
-      </c>
-      <c r="H376" s="2" t="s">
-        <v>6035</v>
-      </c>
-      <c r="I376" s="2" t="s">
-        <v>6026</v>
-      </c>
-      <c r="J376" s="2" t="s">
-        <v>6036</v>
-      </c>
-      <c r="K376" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="L376" s="2" t="s">
-        <v>6037</v>
-      </c>
-      <c r="M376" s="2" t="s">
-        <v>6034</v>
-      </c>
-      <c r="O376" s="2" t="s">
-        <v>6038</v>
-      </c>
-      <c r="P376" s="2" t="s">
-        <v>6032</v>
-      </c>
-      <c r="R376" s="2" t="s">
-        <v>6039</v>
-      </c>
       <c r="T376" s="2" t="s">
-        <v>371</v>
+        <v>6031</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="2" t="s">
+        <v>6034</v>
+      </c>
+      <c r="C377" s="2" t="s">
+        <v>6035</v>
+      </c>
+      <c r="D377" s="1" t="s">
+        <v>6036</v>
+      </c>
+      <c r="G377" s="2" t="s">
+        <v>6037</v>
+      </c>
+      <c r="H377" s="2" t="s">
+        <v>6038</v>
+      </c>
+      <c r="I377" s="2" t="s">
+        <v>6029</v>
+      </c>
+      <c r="J377" s="2" t="s">
+        <v>6039</v>
+      </c>
+      <c r="K377" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="L377" s="2" t="s">
         <v>6040</v>
       </c>
-      <c r="C377" s="2" t="s">
+      <c r="M377" s="2" t="s">
+        <v>6037</v>
+      </c>
+      <c r="O377" s="2" t="s">
         <v>6041</v>
       </c>
-      <c r="D377" s="1" t="s">
+      <c r="P377" s="2" t="s">
+        <v>6035</v>
+      </c>
+      <c r="R377" s="2" t="s">
         <v>6042</v>
       </c>
-      <c r="F377" s="2" t="s">
+      <c r="T377" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A378" s="2" t="s">
         <v>6043</v>
       </c>
-      <c r="G377" s="2" t="s">
+      <c r="C378" s="2" t="s">
         <v>6044</v>
       </c>
-      <c r="H377" s="2" t="s">
+      <c r="D378" s="1" t="s">
         <v>6045</v>
       </c>
-      <c r="I377" s="2" t="s">
+      <c r="F378" s="2" t="s">
         <v>6046</v>
       </c>
-      <c r="J377" s="2" t="s">
+      <c r="G378" s="2" t="s">
         <v>6047</v>
       </c>
-      <c r="K377" s="2" t="s">
+      <c r="H378" s="2" t="s">
         <v>6048</v>
       </c>
-      <c r="L377" s="2" t="s">
+      <c r="I378" s="2" t="s">
         <v>6049</v>
       </c>
-      <c r="M377" s="2" t="s">
+      <c r="J378" s="2" t="s">
         <v>6050</v>
       </c>
-      <c r="O377" s="2" t="s">
+      <c r="K378" s="2" t="s">
         <v>6051</v>
       </c>
-      <c r="P377" s="2" t="s">
+      <c r="L378" s="2" t="s">
         <v>6052</v>
       </c>
-      <c r="R377" s="2" t="s">
+      <c r="M378" s="2" t="s">
         <v>6053</v>
       </c>
-      <c r="T377" s="2" t="s">
+      <c r="O378" s="2" t="s">
         <v>6054</v>
       </c>
+      <c r="P378" s="2" t="s">
+        <v>6055</v>
+      </c>
+      <c r="R378" s="2" t="s">
+        <v>6056</v>
+      </c>
+      <c r="T378" s="2" t="s">
+        <v>6057</v>
+      </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="A1:A1048576">
+  <conditionalFormatting sqref="A340:A1048576 A1:A338">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>